<commit_message>
Atualiza catalogo via planilha Excel
</commit_message>
<xml_diff>
--- a/admin_scaffold/admin/ingredients_master.xlsx
+++ b/admin_scaffold/admin/ingredients_master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sorvetes\admin_scaffold\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B65879F8-E53A-4F33-AB22-C7B80F4E3368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557074E4-BAD9-42F0-A482-F49719ACE4A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28875" yWindow="300" windowWidth="20610" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="142">
   <si>
     <t>id</t>
   </si>
@@ -154,6 +154,24 @@
     <t>coco_polpa</t>
   </si>
   <si>
+    <t>acucar_sacarose</t>
+  </si>
+  <si>
+    <t>glicose_mel_equiv</t>
+  </si>
+  <si>
+    <t>gemas</t>
+  </si>
+  <si>
+    <t>estabilizante_base</t>
+  </si>
+  <si>
+    <t>emulsificante_base</t>
+  </si>
+  <si>
+    <t>agua_polpa</t>
+  </si>
+  <si>
     <t>Leite integral</t>
   </si>
   <si>
@@ -241,6 +259,24 @@
     <t>Polpa de coco (Coco-da-Baía)</t>
   </si>
   <si>
+    <t>Açúcar (sacarose)</t>
+  </si>
+  <si>
+    <t>Glicose/mel (equiv.)</t>
+  </si>
+  <si>
+    <t>Gemas</t>
+  </si>
+  <si>
+    <t>Estabilizante</t>
+  </si>
+  <si>
+    <t>Emulsificante</t>
+  </si>
+  <si>
+    <t>Água/Polpa</t>
+  </si>
+  <si>
     <t>dairy</t>
   </si>
   <si>
@@ -280,6 +316,18 @@
     <t>fruit_pulp</t>
   </si>
   <si>
+    <t>sweetener</t>
+  </si>
+  <si>
+    <t>egg</t>
+  </si>
+  <si>
+    <t>additive</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
     <t>milk</t>
   </si>
   <si>
@@ -292,6 +340,9 @@
     <t>soy</t>
   </si>
   <si>
+    <t>none</t>
+  </si>
+  <si>
     <t>Valores típicos Brasil; ajuste conforme rótulo.</t>
   </si>
   <si>
@@ -371,6 +422,24 @@
   </si>
   <si>
     <t>Valores médios da polpa fresca de coco-da-Baía.</t>
+  </si>
+  <si>
+    <t>Valor típico de sacarose refinada.</t>
+  </si>
+  <si>
+    <t>Aproximação de glicose líquida/mel.</t>
+  </si>
+  <si>
+    <t>Base para receitas custard.</t>
+  </si>
+  <si>
+    <t>Mistura de gomas e mono/di-glicerídeos.</t>
+  </si>
+  <si>
+    <t>Base sintética para sorvetes.</t>
+  </si>
+  <si>
+    <t>Água ou polpa de fruta natural.</t>
   </si>
   <si>
     <t>1.0.0</t>
@@ -744,11 +813,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="57.5703125" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -802,10 +878,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="D2">
         <v>3.2</v>
@@ -823,19 +899,19 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="J2" t="b">
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="L2" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O2" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -843,10 +919,10 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="D3">
         <v>35</v>
@@ -864,19 +940,19 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="J3" t="b">
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="L3" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O3" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -884,10 +960,10 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="D4">
         <v>17</v>
@@ -905,19 +981,19 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="J4" t="b">
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="L4" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O4" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -925,10 +1001,10 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="D5">
         <v>26</v>
@@ -946,19 +1022,19 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="J5" t="b">
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="L5" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O5" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -966,10 +1042,10 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -987,19 +1063,19 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="J6" t="b">
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="L6" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O6" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1007,10 +1083,10 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="D7">
         <v>8</v>
@@ -1028,19 +1104,19 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="J7" t="b">
         <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="L7" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O7" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -1048,10 +1124,10 @@
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1072,13 +1148,13 @@
         <v>1</v>
       </c>
       <c r="K8" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="L8" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O8" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1086,10 +1162,10 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1110,13 +1186,13 @@
         <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="L9" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O9" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -1124,10 +1200,10 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1148,13 +1224,13 @@
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="L10" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O10" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -1162,10 +1238,10 @@
         <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1186,13 +1262,13 @@
         <v>1</v>
       </c>
       <c r="K11" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="L11" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O11" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -1200,10 +1276,10 @@
         <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1224,13 +1300,13 @@
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="L12" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O12" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -1238,10 +1314,10 @@
         <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="D13">
         <v>22</v>
@@ -1262,13 +1338,13 @@
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="L13" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O13" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -1276,10 +1352,10 @@
         <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="D14">
         <v>42</v>
@@ -1300,13 +1376,13 @@
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="L14" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O14" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -1314,10 +1390,10 @@
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="D15">
         <v>32</v>
@@ -1338,13 +1414,13 @@
         <v>1</v>
       </c>
       <c r="K15" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="L15" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O15" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -1352,10 +1428,10 @@
         <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C16" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="D16">
         <v>45</v>
@@ -1373,19 +1449,19 @@
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="J16" t="b">
         <v>1</v>
       </c>
       <c r="K16" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="L16" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O16" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -1393,10 +1469,10 @@
         <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C17" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="D17">
         <v>60</v>
@@ -1414,19 +1490,19 @@
         <v>1</v>
       </c>
       <c r="I17" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="J17" t="b">
         <v>1</v>
       </c>
       <c r="K17" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="L17" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O17" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -1434,10 +1510,10 @@
         <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="D18">
         <v>50</v>
@@ -1455,19 +1531,19 @@
         <v>1</v>
       </c>
       <c r="I18" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="J18" t="b">
         <v>1</v>
       </c>
       <c r="K18" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="L18" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O18" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -1475,10 +1551,10 @@
         <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C19" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1499,13 +1575,13 @@
         <v>1</v>
       </c>
       <c r="K19" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="L19" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O19" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1513,10 +1589,10 @@
         <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1537,13 +1613,13 @@
         <v>1</v>
       </c>
       <c r="K20" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="L20" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O20" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -1551,10 +1627,10 @@
         <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C21" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1572,19 +1648,19 @@
         <v>1</v>
       </c>
       <c r="I21" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="J21" t="b">
         <v>1</v>
       </c>
       <c r="K21" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="L21" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O21" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -1592,10 +1668,10 @@
         <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1616,13 +1692,13 @@
         <v>1</v>
       </c>
       <c r="K22" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="L22" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O22" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -1630,10 +1706,10 @@
         <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C23" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="D23">
         <v>17</v>
@@ -1651,19 +1727,19 @@
         <v>1</v>
       </c>
       <c r="I23" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="J23" t="b">
         <v>1</v>
       </c>
       <c r="K23" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="L23" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O23" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -1671,10 +1747,10 @@
         <v>37</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C24" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="D24">
         <v>0.6</v>
@@ -1695,13 +1771,13 @@
         <v>1</v>
       </c>
       <c r="K24" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="L24" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O24" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -1709,10 +1785,10 @@
         <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C25" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="D25">
         <v>0.5</v>
@@ -1733,13 +1809,13 @@
         <v>1</v>
       </c>
       <c r="K25" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="L25" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O25" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -1747,10 +1823,10 @@
         <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C26" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="D26">
         <v>0.7</v>
@@ -1771,13 +1847,13 @@
         <v>1</v>
       </c>
       <c r="K26" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="L26" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O26" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -1785,10 +1861,10 @@
         <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C27" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="D27">
         <v>0.4</v>
@@ -1809,13 +1885,13 @@
         <v>1</v>
       </c>
       <c r="K27" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="L27" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O27" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -1823,10 +1899,10 @@
         <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C28" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="D28">
         <v>0.6</v>
@@ -1847,13 +1923,13 @@
         <v>1</v>
       </c>
       <c r="K28" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="L28" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O28" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -1861,10 +1937,10 @@
         <v>42</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C29" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="D29">
         <v>0.2</v>
@@ -1885,13 +1961,13 @@
         <v>1</v>
       </c>
       <c r="K29" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="L29" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O29" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -1899,10 +1975,10 @@
         <v>43</v>
       </c>
       <c r="B30" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C30" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="D30">
         <v>33</v>
@@ -1911,7 +1987,7 @@
         <v>6</v>
       </c>
       <c r="F30">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G30">
         <v>0.95</v>
@@ -1920,19 +1996,265 @@
         <v>1</v>
       </c>
       <c r="I30" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="J30" t="b">
         <v>1</v>
       </c>
       <c r="K30" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="L30" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="O30" t="s">
-        <v>118</v>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>100</v>
+      </c>
+      <c r="F31">
+        <v>100</v>
+      </c>
+      <c r="G31">
+        <v>1.59</v>
+      </c>
+      <c r="H31" t="b">
+        <v>1</v>
+      </c>
+      <c r="I31" t="s">
+        <v>106</v>
+      </c>
+      <c r="J31" t="b">
+        <v>1</v>
+      </c>
+      <c r="K31" t="s">
+        <v>134</v>
+      </c>
+      <c r="L31" t="s">
+        <v>140</v>
+      </c>
+      <c r="O31" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>80</v>
+      </c>
+      <c r="F32">
+        <v>80</v>
+      </c>
+      <c r="G32">
+        <v>1.45</v>
+      </c>
+      <c r="H32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" t="s">
+        <v>106</v>
+      </c>
+      <c r="J32" t="b">
+        <v>1</v>
+      </c>
+      <c r="K32" t="s">
+        <v>135</v>
+      </c>
+      <c r="L32" t="s">
+        <v>140</v>
+      </c>
+      <c r="O32" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" t="s">
+        <v>99</v>
+      </c>
+      <c r="D33">
+        <v>30</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>50</v>
+      </c>
+      <c r="G33">
+        <v>1.03</v>
+      </c>
+      <c r="H33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I33" t="s">
+        <v>99</v>
+      </c>
+      <c r="J33" t="b">
+        <v>1</v>
+      </c>
+      <c r="K33" t="s">
+        <v>136</v>
+      </c>
+      <c r="L33" t="s">
+        <v>140</v>
+      </c>
+      <c r="O33" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>100</v>
+      </c>
+      <c r="G34">
+        <v>0.8</v>
+      </c>
+      <c r="H34" t="b">
+        <v>1</v>
+      </c>
+      <c r="I34" t="s">
+        <v>106</v>
+      </c>
+      <c r="J34" t="b">
+        <v>1</v>
+      </c>
+      <c r="K34" t="s">
+        <v>137</v>
+      </c>
+      <c r="L34" t="s">
+        <v>140</v>
+      </c>
+      <c r="O34" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" t="s">
+        <v>100</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>100</v>
+      </c>
+      <c r="G35">
+        <v>0.8</v>
+      </c>
+      <c r="H35" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35" t="s">
+        <v>106</v>
+      </c>
+      <c r="J35" t="b">
+        <v>1</v>
+      </c>
+      <c r="K35" t="s">
+        <v>138</v>
+      </c>
+      <c r="L35" t="s">
+        <v>140</v>
+      </c>
+      <c r="O35" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" t="s">
+        <v>84</v>
+      </c>
+      <c r="C36" t="s">
+        <v>101</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36" t="b">
+        <v>1</v>
+      </c>
+      <c r="I36" t="s">
+        <v>106</v>
+      </c>
+      <c r="J36" t="b">
+        <v>1</v>
+      </c>
+      <c r="K36" t="s">
+        <v>139</v>
+      </c>
+      <c r="L36" t="s">
+        <v>140</v>
+      </c>
+      <c r="O36" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>